<commit_message>
Fixed "Pollutant Sector Other.xlsx".
</commit_message>
<xml_diff>
--- a/Data/Mappings/Pollutant Sector Other.xlsx
+++ b/Data/Mappings/Pollutant Sector Other.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2265" yWindow="0" windowWidth="23040" windowHeight="9150"/>
+    <workbookView xWindow="3375" yWindow="0" windowWidth="23040" windowHeight="9150"/>
   </bookViews>
   <sheets>
     <sheet name="Pollutant Source Other" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="37">
   <si>
     <t>CESI Sector</t>
   </si>
@@ -341,8 +341,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Pollutant_Source_Other" displayName="Pollutant_Source_Other" ref="A2:S16" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A2:S16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Pollutant_Source_Other" displayName="Pollutant_Source_Other" ref="A2:S15" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A2:S15">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -651,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S16"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,76 +993,50 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14">
-        <v>4</v>
-      </c>
-      <c r="D14">
-        <v>4</v>
-      </c>
-      <c r="E14">
-        <v>3</v>
-      </c>
-      <c r="F14">
-        <v>3</v>
-      </c>
-      <c r="G14">
-        <v>3</v>
-      </c>
-      <c r="H14">
-        <v>3</v>
-      </c>
-      <c r="I14">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="L14" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="G15">
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="K15" t="s">
+        <v>36</v>
       </c>
       <c r="L15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16">
-        <v>5</v>
-      </c>
-      <c r="D16">
-        <v>2</v>
-      </c>
-      <c r="E16">
-        <v>4</v>
-      </c>
-      <c r="F16">
-        <v>4</v>
-      </c>
-      <c r="G16">
-        <v>4</v>
-      </c>
-      <c r="H16">
-        <v>4</v>
-      </c>
-      <c r="J16">
-        <v>2</v>
-      </c>
-      <c r="K16" t="s">
-        <v>36</v>
-      </c>
-      <c r="L16" t="s">
-        <v>36</v>
-      </c>
-      <c r="N16" t="s">
-        <v>36</v>
-      </c>
-      <c r="R16" t="s">
-        <v>36</v>
-      </c>
-      <c r="S16" t="s">
+      <c r="N15" t="s">
+        <v>36</v>
+      </c>
+      <c r="R15" t="s">
+        <v>36</v>
+      </c>
+      <c r="S15" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>